<commit_message>
Implemented spreadsheet validate service for tsv
</commit_message>
<xml_diff>
--- a/webtools/tests/data/ExcelMultipleSheets.xlsx
+++ b/webtools/tests/data/ExcelMultipleSheets.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\HEDPython\hed-python\hedweb\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\HEDPython\hed-python\webtools\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="LKT Events" sheetId="1" r:id="rId1"/>
-    <sheet name="PVT Events" sheetId="2" r:id="rId2"/>
-    <sheet name="DAS Events" sheetId="3" r:id="rId3"/>
+    <sheet name="LKT 8Beta3" sheetId="4" r:id="rId1"/>
+    <sheet name="LKT Events" sheetId="1" r:id="rId2"/>
+    <sheet name="PVT Events" sheetId="2" r:id="rId3"/>
+    <sheet name="DAS Events" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>Event code</t>
   </si>
@@ -243,6 +244,21 @@
   </si>
   <si>
     <t>DriverStartsToCorrect</t>
+  </si>
+  <si>
+    <t>Experiment-control, Experimental-stimulus, (Controller-agent, (Operate, Car, (Turn, Leftward)))</t>
+  </si>
+  <si>
+    <t>Experiment-control, Experimental-stimulus, (Controller-agent, (Operate, Car, (Turn, Rightward)))</t>
+  </si>
+  <si>
+    <t>Agent-action, Participant-response, (Halt, Correction)</t>
+  </si>
+  <si>
+    <t>Subject completes response to perturbation having steered the vehicle back to the center of the lane. Normally this would be tagged with temporal scope, but avoiding definitions here.</t>
+  </si>
+  <si>
+    <t>Agent-action, Participant-response, Correction, ((Human-agent, Experimental-participant), (Modify, (Car, Direction)))</t>
   </si>
 </sst>
 </file>
@@ -661,7 +677,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -690,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="58.3">
+    <row r="2" spans="1:5" ht="43.75">
       <c r="A2" s="1">
         <v>251</v>
       </c>
@@ -704,10 +720,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="58.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.75">
       <c r="A3" s="1">
         <v>252</v>
       </c>
@@ -721,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="47.05" customHeight="1">
@@ -738,10 +754,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="58.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.75">
       <c r="A5" s="1">
         <v>254</v>
       </c>
@@ -752,10 +768,10 @@
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -765,6 +781,114 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="1" max="1" width="15.3828125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="23.07421875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.3828125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.921875" style="2" customWidth="1"/>
+    <col min="6" max="1026" width="8.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="58.3">
+      <c r="A2" s="1">
+        <v>251</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="58.3">
+      <c r="A3" s="1">
+        <v>252</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="47.05" customHeight="1">
+      <c r="A4" s="1">
+        <v>253</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="58.3">
+      <c r="A5" s="1">
+        <v>254</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -871,7 +995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Eliminated extra functions in the utilities
</commit_message>
<xml_diff>
--- a/webtools/tests/data/ExcelMultipleSheets.xlsx
+++ b/webtools/tests/data/ExcelMultipleSheets.xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="LKT 8Beta3" sheetId="4" r:id="rId1"/>
+    <sheet name="LKT 8HED3" sheetId="4" r:id="rId1"/>
     <sheet name="LKT Events" sheetId="1" r:id="rId2"/>
     <sheet name="PVT Events" sheetId="2" r:id="rId3"/>
     <sheet name="DAS Events" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -258,7 +258,7 @@
     <t>Subject completes response to perturbation having steered the vehicle back to the center of the lane. Normally this would be tagged with temporal scope, but avoiding definitions here.</t>
   </si>
   <si>
-    <t>Agent-action, Participant-response, Correction, ((Human-agent, Experimental-participant), (Modify, (Car, Direction)))</t>
+    <t>Agent-action, Participant-response, Correction, ((Human-agent, Experiment-participant), (Modify, (Car, Direction)))</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>

</xml_diff>

<commit_message>
Moved the action to the top of the pages
</commit_message>
<xml_diff>
--- a/webtools/tests/data/ExcelMultipleSheets.xlsx
+++ b/webtools/tests/data/ExcelMultipleSheets.xlsx
@@ -258,7 +258,7 @@
     <t>Subject completes response to perturbation having steered the vehicle back to the center of the lane. Normally this would be tagged with temporal scope, but avoiding definitions here.</t>
   </si>
   <si>
-    <t>Agent-action, Participant-response, Correction, ((Human-agent, Experiment-participant), (Modify, (Car, Direction)))</t>
+    <t>Agent-action, Participant-response, Correction, ((Human-agent, Experiment-participant), (Modify, (Car,Angle)))</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>

</xml_diff>